<commit_message>
sql queries now account for all selected
</commit_message>
<xml_diff>
--- a/DeliveryPerformance/template/template.xlsx
+++ b/DeliveryPerformance/template/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="8775" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -915,19 +915,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="34" style="1" customWidth="1"/>
@@ -1019,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change template header and select all header
The excel document template header is now yellow. The select all header
is now correctly repainted using getContentPane().repaint(). Whitespaces
and searches without any matches in regex has been fixed
</commit_message>
<xml_diff>
--- a/DeliveryPerformance/template/template.xlsx
+++ b/DeliveryPerformance/template/template.xlsx
@@ -147,7 +147,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,7 +196,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -206,6 +212,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -229,6 +236,12 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -598,29 +611,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabell4" displayName="Tabell4" ref="A1:T1048576" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabell4" displayName="Tabell4" ref="A1:T1048576" totalsRowShown="0" headerRowDxfId="0" dataDxfId="21">
   <autoFilter ref="A1:T1048576"/>
   <tableColumns count="20">
-    <tableColumn id="1" name="Project" dataDxfId="19"/>
-    <tableColumn id="2" name="Client" dataDxfId="18"/>
-    <tableColumn id="3" name="Client Ref." dataDxfId="17"/>
-    <tableColumn id="4" name="Order Nr." dataDxfId="16"/>
-    <tableColumn id="5" name="Order Reg Date" dataDxfId="15"/>
-    <tableColumn id="6" name="Item Nr." dataDxfId="14"/>
-    <tableColumn id="7" name="Client Art. Code" dataDxfId="13"/>
-    <tableColumn id="8" name="Vendor Nr." dataDxfId="12"/>
-    <tableColumn id="9" name="Description" dataDxfId="11"/>
-    <tableColumn id="10" name="Supplier" dataDxfId="10"/>
-    <tableColumn id="11" name="QTY" dataDxfId="9"/>
-    <tableColumn id="12" name="Unit Price" dataDxfId="8"/>
-    <tableColumn id="13" name="Total Price" dataDxfId="7"/>
-    <tableColumn id="14" name="Currency" dataDxfId="6"/>
-    <tableColumn id="15" name="CDD" dataDxfId="5"/>
-    <tableColumn id="16" name="EDD" dataDxfId="4"/>
-    <tableColumn id="17" name="RFI" dataDxfId="3"/>
-    <tableColumn id="18" name="CCD" dataDxfId="2"/>
-    <tableColumn id="19" name="ECD" dataDxfId="1"/>
-    <tableColumn id="20" name="Item Status" dataDxfId="0"/>
+    <tableColumn id="1" name="Project" dataDxfId="20"/>
+    <tableColumn id="2" name="Client" dataDxfId="19"/>
+    <tableColumn id="3" name="Client Ref." dataDxfId="18"/>
+    <tableColumn id="4" name="Order Nr." dataDxfId="17"/>
+    <tableColumn id="5" name="Order Reg Date" dataDxfId="16"/>
+    <tableColumn id="6" name="Item Nr." dataDxfId="15"/>
+    <tableColumn id="7" name="Client Art. Code" dataDxfId="14"/>
+    <tableColumn id="8" name="Vendor Nr." dataDxfId="13"/>
+    <tableColumn id="9" name="Description" dataDxfId="12"/>
+    <tableColumn id="10" name="Supplier" dataDxfId="11"/>
+    <tableColumn id="11" name="QTY" dataDxfId="10"/>
+    <tableColumn id="12" name="Unit Price" dataDxfId="9"/>
+    <tableColumn id="13" name="Total Price" dataDxfId="8"/>
+    <tableColumn id="14" name="Currency" dataDxfId="7"/>
+    <tableColumn id="15" name="CDD" dataDxfId="6"/>
+    <tableColumn id="16" name="EDD" dataDxfId="5"/>
+    <tableColumn id="17" name="RFI" dataDxfId="4"/>
+    <tableColumn id="18" name="CCD" dataDxfId="3"/>
+    <tableColumn id="19" name="ECD" dataDxfId="2"/>
+    <tableColumn id="20" name="Item Status" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -916,7 +929,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -944,65 +957,65 @@
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="13" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Currencies sorted in excel report
</commit_message>
<xml_diff>
--- a/DeliveryPerformance/template/template.xlsx
+++ b/DeliveryPerformance/template/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="8775"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="8775" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Project</t>
   </si>
@@ -87,12 +87,6 @@
   </si>
   <si>
     <t>Item [%]</t>
-  </si>
-  <si>
-    <t>Total Value [EUR]:</t>
-  </si>
-  <si>
-    <t>Total Value [NOK]:</t>
   </si>
   <si>
     <t>Delivered to FA:</t>
@@ -196,7 +190,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -204,9 +198,7 @@
     <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -236,369 +228,369 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -611,29 +603,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabell4" displayName="Tabell4" ref="A1:T1048576" totalsRowShown="0" headerRowDxfId="0" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabell4" displayName="Tabell4" ref="A1:T1048576" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:T1048576"/>
   <tableColumns count="20">
-    <tableColumn id="1" name="Project" dataDxfId="20"/>
-    <tableColumn id="2" name="Client" dataDxfId="19"/>
-    <tableColumn id="3" name="Client Ref." dataDxfId="18"/>
-    <tableColumn id="4" name="Order Nr." dataDxfId="17"/>
-    <tableColumn id="5" name="Order Reg Date" dataDxfId="16"/>
-    <tableColumn id="6" name="Item Nr." dataDxfId="15"/>
-    <tableColumn id="7" name="Client Art. Code" dataDxfId="14"/>
-    <tableColumn id="8" name="Vendor Nr." dataDxfId="13"/>
-    <tableColumn id="9" name="Description" dataDxfId="12"/>
-    <tableColumn id="10" name="Supplier" dataDxfId="11"/>
-    <tableColumn id="11" name="QTY" dataDxfId="10"/>
-    <tableColumn id="12" name="Unit Price" dataDxfId="9"/>
-    <tableColumn id="13" name="Total Price" dataDxfId="8"/>
-    <tableColumn id="14" name="Currency" dataDxfId="7"/>
-    <tableColumn id="15" name="CDD" dataDxfId="6"/>
-    <tableColumn id="16" name="EDD" dataDxfId="5"/>
-    <tableColumn id="17" name="RFI" dataDxfId="4"/>
-    <tableColumn id="18" name="CCD" dataDxfId="3"/>
-    <tableColumn id="19" name="ECD" dataDxfId="2"/>
-    <tableColumn id="20" name="Item Status" dataDxfId="1"/>
+    <tableColumn id="1" name="Project" dataDxfId="19"/>
+    <tableColumn id="2" name="Client" dataDxfId="18"/>
+    <tableColumn id="3" name="Client Ref." dataDxfId="17"/>
+    <tableColumn id="4" name="Order Nr." dataDxfId="16"/>
+    <tableColumn id="5" name="Order Reg Date" dataDxfId="15"/>
+    <tableColumn id="6" name="Item Nr." dataDxfId="14"/>
+    <tableColumn id="7" name="Client Art. Code" dataDxfId="13"/>
+    <tableColumn id="8" name="Vendor Nr." dataDxfId="12"/>
+    <tableColumn id="9" name="Description" dataDxfId="11"/>
+    <tableColumn id="10" name="Supplier" dataDxfId="10"/>
+    <tableColumn id="11" name="QTY" dataDxfId="9"/>
+    <tableColumn id="12" name="Unit Price" dataDxfId="8"/>
+    <tableColumn id="13" name="Total Price" dataDxfId="7"/>
+    <tableColumn id="14" name="Currency" dataDxfId="6"/>
+    <tableColumn id="15" name="CDD" dataDxfId="5"/>
+    <tableColumn id="16" name="EDD" dataDxfId="4"/>
+    <tableColumn id="17" name="RFI" dataDxfId="3"/>
+    <tableColumn id="18" name="CCD" dataDxfId="2"/>
+    <tableColumn id="19" name="ECD" dataDxfId="1"/>
+    <tableColumn id="20" name="Item Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -928,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -957,65 +949,65 @@
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1030,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E11"/>
+  <dimension ref="A4:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,67 +1053,49 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="5"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="5"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Total value now in NOK only
</commit_message>
<xml_diff>
--- a/DeliveryPerformance/template/template.xlsx
+++ b/DeliveryPerformance/template/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="8775" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Project</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>Items delivered outside Scope</t>
+  </si>
+  <si>
+    <t>Total Value [EUR]:</t>
+  </si>
+  <si>
+    <t>Total Value [NOK]:</t>
+  </si>
+  <si>
+    <t>EX-Rate</t>
   </si>
 </sst>
 </file>
@@ -190,7 +199,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -205,13 +214,32 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Prosent" xfId="2" builtinId="5"/>
     <cellStyle name="Valuta" xfId="1" builtinId="4"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -603,23 +631,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabell4" displayName="Tabell4" ref="A1:T1048576" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:T1048576"/>
-  <tableColumns count="20">
-    <tableColumn id="1" name="Project" dataDxfId="19"/>
-    <tableColumn id="2" name="Client" dataDxfId="18"/>
-    <tableColumn id="3" name="Client Ref." dataDxfId="17"/>
-    <tableColumn id="4" name="Order Nr." dataDxfId="16"/>
-    <tableColumn id="5" name="Order Reg Date" dataDxfId="15"/>
-    <tableColumn id="6" name="Item Nr." dataDxfId="14"/>
-    <tableColumn id="7" name="Client Art. Code" dataDxfId="13"/>
-    <tableColumn id="8" name="Vendor Nr." dataDxfId="12"/>
-    <tableColumn id="9" name="Description" dataDxfId="11"/>
-    <tableColumn id="10" name="Supplier" dataDxfId="10"/>
-    <tableColumn id="11" name="QTY" dataDxfId="9"/>
-    <tableColumn id="12" name="Unit Price" dataDxfId="8"/>
-    <tableColumn id="13" name="Total Price" dataDxfId="7"/>
-    <tableColumn id="14" name="Currency" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabell4" displayName="Tabell4" ref="A1:U1048576" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:U1048576"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="Project" dataDxfId="20"/>
+    <tableColumn id="2" name="Client" dataDxfId="19"/>
+    <tableColumn id="3" name="Client Ref." dataDxfId="18"/>
+    <tableColumn id="4" name="Order Nr." dataDxfId="17"/>
+    <tableColumn id="5" name="Order Reg Date" dataDxfId="16"/>
+    <tableColumn id="6" name="Item Nr." dataDxfId="15"/>
+    <tableColumn id="7" name="Client Art. Code" dataDxfId="14"/>
+    <tableColumn id="8" name="Vendor Nr." dataDxfId="13"/>
+    <tableColumn id="9" name="Description" dataDxfId="12"/>
+    <tableColumn id="10" name="Supplier" dataDxfId="11"/>
+    <tableColumn id="11" name="QTY" dataDxfId="10"/>
+    <tableColumn id="12" name="Unit Price" dataDxfId="9"/>
+    <tableColumn id="13" name="Total Price" dataDxfId="8"/>
+    <tableColumn id="14" name="Currency" dataDxfId="7"/>
+    <tableColumn id="21" name="EX-Rate" dataDxfId="6"/>
     <tableColumn id="15" name="CDD" dataDxfId="5"/>
     <tableColumn id="16" name="EDD" dataDxfId="4"/>
     <tableColumn id="17" name="RFI" dataDxfId="3"/>
@@ -918,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -939,17 +968,17 @@
     <col min="11" max="11" width="11.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="15" width="11.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -993,21 +1022,24 @@
         <v>13</v>
       </c>
       <c r="O1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1022,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E9"/>
+  <dimension ref="A4:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,49 +1085,67 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>24</v>
+      <c r="A5" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>25</v>
+      <c r="A6" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="5"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Moved total value column and added color
</commit_message>
<xml_diff>
--- a/DeliveryPerformance/template/template.xlsx
+++ b/DeliveryPerformance/template/template.xlsx
@@ -53,9 +53,6 @@
     <t>Unit Price</t>
   </si>
   <si>
-    <t>Total Price</t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>EX-Rate</t>
+  </si>
+  <si>
+    <t>Total Value</t>
   </si>
 </sst>
 </file>
@@ -239,6 +239,12 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -646,15 +652,15 @@
     <tableColumn id="10" name="Supplier" dataDxfId="11"/>
     <tableColumn id="11" name="QTY" dataDxfId="10"/>
     <tableColumn id="12" name="Unit Price" dataDxfId="9"/>
-    <tableColumn id="13" name="Total Price" dataDxfId="8"/>
-    <tableColumn id="14" name="Currency" dataDxfId="7"/>
-    <tableColumn id="21" name="EX-Rate" dataDxfId="6"/>
-    <tableColumn id="15" name="CDD" dataDxfId="5"/>
-    <tableColumn id="16" name="EDD" dataDxfId="4"/>
-    <tableColumn id="17" name="RFI" dataDxfId="3"/>
-    <tableColumn id="18" name="CCD" dataDxfId="2"/>
-    <tableColumn id="19" name="ECD" dataDxfId="1"/>
-    <tableColumn id="20" name="Item Status" dataDxfId="0"/>
+    <tableColumn id="13" name="Currency" dataDxfId="8"/>
+    <tableColumn id="14" name="EX-Rate" dataDxfId="7"/>
+    <tableColumn id="21" name="CDD" dataDxfId="6"/>
+    <tableColumn id="15" name="EDD" dataDxfId="5"/>
+    <tableColumn id="16" name="RFI" dataDxfId="4"/>
+    <tableColumn id="17" name="CCD" dataDxfId="3"/>
+    <tableColumn id="18" name="ECD" dataDxfId="2"/>
+    <tableColumn id="19" name="Item Status" dataDxfId="1"/>
+    <tableColumn id="20" name="Total Value" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -949,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -973,8 +979,7 @@
     <col min="17" max="17" width="12" style="1" customWidth="1"/>
     <col min="18" max="18" width="12.140625" style="1" customWidth="1"/>
     <col min="19" max="19" width="11.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" style="1" customWidth="1"/>
+    <col min="20" max="21" width="11.85546875" style="1" customWidth="1"/>
     <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1019,10 +1024,10 @@
         <v>12</v>
       </c>
       <c r="N1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>31</v>
       </c>
       <c r="P1" s="11" t="s">
         <v>14</v>
@@ -1040,7 +1045,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1072,21 +1077,21 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5"/>
@@ -1095,7 +1100,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="5"/>
@@ -1104,7 +1109,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
@@ -1113,7 +1118,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
@@ -1122,7 +1127,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="5"/>
@@ -1131,7 +1136,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
@@ -1140,7 +1145,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="5"/>

</xml_diff>

<commit_message>
Started to work on the "Mill" sheet
</commit_message>
<xml_diff>
--- a/DeliveryPerformance/template/template.xlsx
+++ b/DeliveryPerformance/template/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="8775" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1197,9 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1297,9 +1295,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a graph to the delay sheet and used data
</commit_message>
<xml_diff>
--- a/DeliveryPerformance/template/template.xlsx
+++ b/DeliveryPerformance/template/template.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="8775"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="8775" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="Project" sheetId="4" r:id="rId2"/>
     <sheet name="Mill" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O27"/>
 </workbook>
 </file>
 
@@ -968,7 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1088,7 +1089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>